<commit_message>
update summary experimental results for multiple bugs
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/Summary/All/multiple_bugs_2bug.xlsx
+++ b/experiment_results/SBFL_ONLY/Summary/All/multiple_bugs_2bug.xlsx
@@ -420,7 +420,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.03336572724327826</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1326530612244898</v>
+        <v>0.1328478964401294</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -436,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2103984450923227</v>
+        <v>0.2105177993527508</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -444,7 +444,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.2623906705539358</v>
+        <v>0.2624595469255664</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -452,7 +452,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.329770003239391</v>
+        <v>0.3297734627831715</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -463,7 +463,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.06705539358600583</v>
+        <v>0.06699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -471,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2643343051506317</v>
+        <v>0.2650485436893204</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.402332361516035</v>
+        <v>0.4029126213592233</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.4742468415937804</v>
+        <v>0.4747572815533981</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.5587949465500486</v>
+        <v>0.5592233009708738</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>6.717201166180758</v>
+        <v>6.712621359223301</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -511,7 +511,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>59.11273080660835</v>
+        <v>59.06310679611651</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08471007450599287</v>
+        <v>0.08462783171521035</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2447359896339488</v>
+        <v>0.2449838187702265</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -562,7 +562,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3986070618723679</v>
+        <v>0.398705501618123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -570,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4782960803368966</v>
+        <v>0.4783171521035599</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -578,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5361192095885974</v>
+        <v>0.536084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1700680272108843</v>
+        <v>0.1699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -597,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4878522837706511</v>
+        <v>0.4883495145631068</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -605,7 +605,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7842565597667639</v>
+        <v>0.7844660194174757</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.880466472303207</v>
+        <v>0.8805825242718447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -621,7 +621,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9212827988338192</v>
+        <v>0.9213592233009709</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -629,7 +629,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.382896015549077</v>
+        <v>3.381553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -637,7 +637,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>56.86297376093295</v>
+        <v>56.81553398058252</v>
       </c>
     </row>
   </sheetData>
@@ -672,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08519598315516681</v>
+        <v>0.08511326860841423</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -680,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2457078069322967</v>
+        <v>0.2459546925566343</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -688,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.398121153223194</v>
+        <v>0.3982200647249191</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -696,7 +696,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4782960803368966</v>
+        <v>0.4783171521035599</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -704,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5327178490443797</v>
+        <v>0.5326860841423949</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1710398445092323</v>
+        <v>0.170873786407767</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -723,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4897959183673469</v>
+        <v>0.4902912621359223</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -731,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.782312925170068</v>
+        <v>0.7825242718446602</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8775510204081632</v>
+        <v>0.8776699029126214</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -747,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9115646258503401</v>
+        <v>0.9116504854368932</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -755,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.435374149659864</v>
+        <v>3.433980582524272</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -763,7 +763,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>51.1175898931001</v>
+        <v>51.0757281553398</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08438613540654356</v>
+        <v>0.0843042071197411</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -806,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2444120505344995</v>
+        <v>0.2446601941747573</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3958535795270489</v>
+        <v>0.3959546925566343</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -822,7 +822,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.471169420149012</v>
+        <v>0.4711974110032363</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -830,7 +830,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.526077097505669</v>
+        <v>0.526051779935275</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1690962099125364</v>
+        <v>0.1689320388349514</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -849,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4868804664723032</v>
+        <v>0.487378640776699</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7774538386783285</v>
+        <v>0.7776699029126214</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -865,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8629737609329446</v>
+        <v>0.8631067961165049</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -873,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.8979591836734694</v>
+        <v>0.8980582524271845</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -881,7 +881,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>6.572400388726919</v>
+        <v>6.567961165048544</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -889,7 +889,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>74.86783284742468</v>
+        <v>74.80291262135923</v>
       </c>
     </row>
   </sheetData>
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08438613540654356</v>
+        <v>0.0843042071197411</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2444120505344995</v>
+        <v>0.2446601941747573</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -940,7 +940,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3958535795270489</v>
+        <v>0.3959546925566343</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -948,7 +948,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.471169420149012</v>
+        <v>0.4711974110032363</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -956,7 +956,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.526077097505669</v>
+        <v>0.526051779935275</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1690962099125364</v>
+        <v>0.1689320388349514</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -975,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4868804664723032</v>
+        <v>0.487378640776699</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -983,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7774538386783285</v>
+        <v>0.7776699029126214</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -991,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8629737609329446</v>
+        <v>0.8631067961165049</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -999,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.8979591836734694</v>
+        <v>0.8980582524271845</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1007,7 +1007,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>6.572400388726919</v>
+        <v>6.567961165048544</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1015,7 +1015,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>74.86783284742468</v>
+        <v>74.80291262135923</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08519598315516681</v>
+        <v>0.08511326860841423</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1058,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2466796242306447</v>
+        <v>0.2469255663430421</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1066,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.4058956916099773</v>
+        <v>0.4059870550161812</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1074,7 +1074,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4807256235827664</v>
+        <v>0.4807443365695793</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1082,7 +1082,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5375769355361193</v>
+        <v>0.5375404530744338</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1093,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1710398445092323</v>
+        <v>0.170873786407767</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1101,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4917395529640428</v>
+        <v>0.4922330097087378</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1109,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7998056365403304</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1117,7 +1117,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8940719144800777</v>
+        <v>0.8941747572815534</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1125,7 +1125,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.93488824101069</v>
+        <v>0.9349514563106797</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1133,7 +1133,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.134110787172012</v>
+        <v>3.133009708737864</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>52.2798833819242</v>
+        <v>52.2368932038835</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05183025591188857</v>
+        <v>0.0517799352750809</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1184,7 +1184,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1681243926141885</v>
+        <v>0.1684466019417476</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1192,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2889536767087787</v>
+        <v>0.28915857605178</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1200,7 +1200,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3424036281179137</v>
+        <v>0.3425566343042071</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1208,7 +1208,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3671849692257855</v>
+        <v>0.3673139158576052</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1039844509232264</v>
+        <v>0.1038834951456311</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1227,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.337220602526725</v>
+        <v>0.3378640776699029</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1235,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5772594752186589</v>
+        <v>0.5776699029126213</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1243,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6754130223517979</v>
+        <v>0.6757281553398058</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.7142857142857143</v>
+        <v>0.7145631067961165</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1259,7 +1259,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>4.89310009718173</v>
+        <v>4.890291262135922</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1267,7 +1267,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>70.40913508260446</v>
+        <v>70.36504854368933</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.00826044703595724</v>
+        <v>0.00825242718446602</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1318,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.03822481373501782</v>
+        <v>0.03818770226537217</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1326,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.0785552316164561</v>
+        <v>0.07880258899676375</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1334,7 +1334,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.1052802073210236</v>
+        <v>0.1055016181229773</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1353,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.01652089407191448</v>
+        <v>0.01650485436893204</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1361,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.07677356656948493</v>
+        <v>0.0766990291262136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1369,7 +1369,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.1574344023323615</v>
+        <v>0.158252427184466</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1377,7 +1377,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.2089407191448008</v>
+        <v>0.2097087378640777</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1385,7 +1385,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>15.73760932944606</v>
+        <v>15.72621359223301</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1393,7 +1393,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>81.23420796890184</v>
+        <v>81.1883495145631</v>
       </c>
     </row>
   </sheetData>
@@ -1428,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1436,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1444,7 +1444,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1460,7 +1460,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1471,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1479,7 +1479,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1487,7 +1487,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1495,7 +1495,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1503,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1511,7 +1511,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1519,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08471007450599287</v>
+        <v>0.08462783171521035</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1562,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2447359896339488</v>
+        <v>0.2449838187702265</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3986070618723679</v>
+        <v>0.398705501618123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1578,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4782960803368966</v>
+        <v>0.4783171521035599</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1586,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5361192095885974</v>
+        <v>0.536084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1700680272108843</v>
+        <v>0.1699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1605,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4878522837706511</v>
+        <v>0.4883495145631068</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7842565597667639</v>
+        <v>0.7844660194174757</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1621,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.880466472303207</v>
+        <v>0.8805825242718447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1629,7 +1629,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9212827988338192</v>
+        <v>0.9213592233009709</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1637,7 +1637,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.382896015549077</v>
+        <v>3.381553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1645,7 +1645,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>56.86297376093295</v>
+        <v>56.81553398058252</v>
       </c>
     </row>
   </sheetData>
@@ -1680,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08471007450599287</v>
+        <v>0.08462783171521035</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2447359896339488</v>
+        <v>0.2449838187702265</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3986070618723679</v>
+        <v>0.398705501618123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1704,7 +1704,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4782960803368966</v>
+        <v>0.4783171521035599</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1712,7 +1712,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5361192095885974</v>
+        <v>0.536084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1723,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1700680272108843</v>
+        <v>0.1699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1731,7 +1731,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4878522837706511</v>
+        <v>0.4883495145631068</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1739,7 +1739,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7842565597667639</v>
+        <v>0.7844660194174757</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1747,7 +1747,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.880466472303207</v>
+        <v>0.8805825242718447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1755,7 +1755,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9212827988338192</v>
+        <v>0.9213592233009709</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1763,7 +1763,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.382896015549077</v>
+        <v>3.381553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1771,7 +1771,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>56.86297376093295</v>
+        <v>56.81553398058252</v>
       </c>
     </row>
   </sheetData>
@@ -1806,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08519598315516681</v>
+        <v>0.08511326860841423</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1814,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2457078069322967</v>
+        <v>0.2459546925566343</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1822,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.4068675089083252</v>
+        <v>0.406957928802589</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1830,7 +1830,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4841269841269841</v>
+        <v>0.4841423948220065</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1838,7 +1838,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5361192095885974</v>
+        <v>0.536084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1849,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1710398445092323</v>
+        <v>0.170873786407767</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1857,7 +1857,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4897959183673469</v>
+        <v>0.4902912621359223</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1865,7 +1865,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.8007774538386784</v>
+        <v>0.8009708737864077</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1873,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.901846452866861</v>
+        <v>0.9019417475728155</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1881,7 +1881,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9339164237123421</v>
+        <v>0.9339805825242719</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1889,7 +1889,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.113702623906705</v>
+        <v>3.112621359223301</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1897,7 +1897,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>57.9757045675413</v>
+        <v>57.92912621359223</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1940,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1948,7 +1948,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1956,7 +1956,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1964,7 +1964,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1975,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1983,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1991,7 +1991,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1999,7 +1999,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2007,7 +2007,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2015,7 +2015,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2023,7 +2023,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -2058,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2066,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2074,7 +2074,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2082,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2090,7 +2090,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2109,7 +2109,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2117,7 +2117,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2125,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2133,7 +2133,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2141,7 +2141,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2149,7 +2149,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2192,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2200,7 +2200,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2208,7 +2208,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2216,7 +2216,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2227,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2235,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2243,7 +2243,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2251,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2259,7 +2259,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2267,7 +2267,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2275,7 +2275,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -2310,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.03563330093942339</v>
+        <v>0.03559870550161812</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2318,7 +2318,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.0973436993845157</v>
+        <v>0.09724919093851132</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2326,7 +2326,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2308066083576288</v>
+        <v>0.2305825242718447</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2334,7 +2334,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3049886621315193</v>
+        <v>0.3051779935275081</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2342,7 +2342,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3487204405571752</v>
+        <v>0.3488673139158576</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2353,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.07191448007774538</v>
+        <v>0.07184466019417475</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2361,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.19533527696793</v>
+        <v>0.1951456310679612</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2369,7 +2369,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.456754130223518</v>
+        <v>0.4563106796116505</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2377,7 +2377,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.586977648202138</v>
+        <v>0.587378640776699</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2385,7 +2385,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6482021379980564</v>
+        <v>0.6485436893203883</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2393,7 +2393,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>6.304178814382896</v>
+        <v>6.301941747572815</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2401,7 +2401,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>62.79786200194363</v>
+        <v>62.74660194174757</v>
       </c>
     </row>
   </sheetData>
@@ -2436,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.0798509880142533</v>
+        <v>0.07977346278317153</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2444,7 +2444,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2150955620343376</v>
+        <v>0.2153721682847897</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2452,7 +2452,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3956916099773242</v>
+        <v>0.3957928802588996</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2460,7 +2460,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4680919987042436</v>
+        <v>0.4681229773462783</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2468,7 +2468,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.518626498218335</v>
+        <v>0.5186084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2479,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1603498542274052</v>
+        <v>0.1601941747572816</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2487,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4285714285714285</v>
+        <v>0.429126213592233</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2495,7 +2495,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7813411078717201</v>
+        <v>0.7815533980582524</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2503,7 +2503,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8882410106899903</v>
+        <v>0.8883495145631068</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2511,7 +2511,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9271137026239067</v>
+        <v>0.9271844660194175</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2519,7 +2519,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.182701652089407</v>
+        <v>3.181553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2527,7 +2527,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>65.15937803692906</v>
+        <v>65.10582524271845</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2570,7 +2570,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2578,7 +2578,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2586,7 +2586,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2594,7 +2594,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2613,7 +2613,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2621,7 +2621,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2629,7 +2629,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2637,7 +2637,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2645,7 +2645,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2653,7 +2653,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -2688,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08098477486232587</v>
+        <v>0.08090614886731391</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2696,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2361516034985423</v>
+        <v>0.2364077669902913</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2704,7 +2704,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3977972141237447</v>
+        <v>0.3978964401294499</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2712,7 +2712,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.470683511499838</v>
+        <v>0.4707119741100324</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2720,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5139293812763199</v>
+        <v>0.5139158576051779</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2731,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1622934888241011</v>
+        <v>0.1621359223300971</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2739,7 +2739,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4732750242954324</v>
+        <v>0.4737864077669903</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2747,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7891156462585034</v>
+        <v>0.7893203883495146</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2755,7 +2755,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8960155490767736</v>
+        <v>0.8961165048543689</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2763,7 +2763,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9329446064139941</v>
+        <v>0.933009708737864</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2771,7 +2771,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>6.302235179786201</v>
+        <v>6.298058252427184</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2779,7 +2779,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>80.09426627793975</v>
+        <v>80.02427184466019</v>
       </c>
     </row>
   </sheetData>
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08471007450599287</v>
+        <v>0.08462783171521035</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2822,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2447359896339488</v>
+        <v>0.2449838187702265</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2830,7 +2830,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3986070618723679</v>
+        <v>0.398705501618123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2838,7 +2838,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4782960803368966</v>
+        <v>0.4783171521035599</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2846,7 +2846,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5361192095885974</v>
+        <v>0.536084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2857,7 +2857,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1700680272108843</v>
+        <v>0.1699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2865,7 +2865,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4878522837706511</v>
+        <v>0.4883495145631068</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2873,7 +2873,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7842565597667639</v>
+        <v>0.7844660194174757</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2881,7 +2881,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.880466472303207</v>
+        <v>0.8805825242718447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2889,7 +2889,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9212827988338192</v>
+        <v>0.9213592233009709</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2897,7 +2897,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.382896015549077</v>
+        <v>3.381553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>56.86297376093295</v>
+        <v>56.81553398058252</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08471007450599287</v>
+        <v>0.08462783171521035</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2948,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2447359896339488</v>
+        <v>0.2449838187702265</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2956,7 +2956,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3986070618723679</v>
+        <v>0.398705501618123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2964,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4782960803368966</v>
+        <v>0.4783171521035599</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2972,7 +2972,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5361192095885974</v>
+        <v>0.536084142394822</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1700680272108843</v>
+        <v>0.1699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2991,7 +2991,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4878522837706511</v>
+        <v>0.4883495145631068</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2999,7 +2999,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7842565597667639</v>
+        <v>0.7844660194174757</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3007,7 +3007,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.880466472303207</v>
+        <v>0.8805825242718447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3015,7 +3015,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9212827988338192</v>
+        <v>0.9213592233009709</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3023,7 +3023,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.382896015549077</v>
+        <v>3.381553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3031,7 +3031,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>56.86297376093295</v>
+        <v>56.81553398058252</v>
       </c>
     </row>
   </sheetData>
@@ -3066,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.0798509880142533</v>
+        <v>0.07977346278317153</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3074,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2150955620343376</v>
+        <v>0.2153721682847897</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3082,7 +3082,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3956916099773242</v>
+        <v>0.3957928802588996</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3090,7 +3090,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4680919987042436</v>
+        <v>0.4681229773462783</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3098,7 +3098,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.518140589569161</v>
+        <v>0.5181229773462784</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3109,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1603498542274052</v>
+        <v>0.1601941747572816</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3117,7 +3117,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4285714285714285</v>
+        <v>0.429126213592233</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3125,7 +3125,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7813411078717201</v>
+        <v>0.7815533980582524</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3133,7 +3133,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8882410106899903</v>
+        <v>0.8883495145631068</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3141,7 +3141,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.9271137026239067</v>
+        <v>0.9271844660194175</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3149,7 +3149,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.182701652089407</v>
+        <v>3.181553398058252</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3157,7 +3157,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>54.53644314868804</v>
+        <v>54.49320388349515</v>
       </c>
     </row>
   </sheetData>
@@ -3192,7 +3192,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.01733074182053774</v>
+        <v>0.01731391585760518</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3200,7 +3200,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.06203433754454163</v>
+        <v>0.06197411003236246</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3208,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.1297376093294461</v>
+        <v>0.1296116504854369</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3216,7 +3216,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.1603498542274052</v>
+        <v>0.1605177993527508</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3224,7 +3224,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.1919339164237124</v>
+        <v>0.1920711974110033</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3235,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.03498542274052478</v>
+        <v>0.03495145631067961</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3243,7 +3243,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.1243926141885325</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3251,7 +3251,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.2604470359572401</v>
+        <v>0.2601941747572816</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3259,7 +3259,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.3206997084548105</v>
+        <v>0.3213592233009709</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3267,7 +3267,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.3722060252672498</v>
+        <v>0.3728155339805825</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3275,7 +3275,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>9.137998056365403</v>
+        <v>9.133009708737864</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3283,7 +3283,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>57.06025267249757</v>
+        <v>57.0378640776699</v>
       </c>
     </row>
   </sheetData>
@@ -3318,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.07839326206673145</v>
+        <v>0.07831715210355987</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3326,7 +3326,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2010042112082928</v>
+        <v>0.201294498381877</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3334,7 +3334,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3786848072562358</v>
+        <v>0.3788025889967637</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3342,7 +3342,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4501133786848072</v>
+        <v>0.4501618122977347</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3350,7 +3350,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.4826692581794622</v>
+        <v>0.4826860841423948</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3361,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1574344023323615</v>
+        <v>0.1572815533980582</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3369,7 +3369,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4003887269193392</v>
+        <v>0.4009708737864078</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3377,7 +3377,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7512147716229349</v>
+        <v>0.7514563106796116</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3385,7 +3385,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8688046647230321</v>
+        <v>0.8689320388349514</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3393,7 +3393,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.8979591836734694</v>
+        <v>0.8980582524271845</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3401,7 +3401,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.745383867832847</v>
+        <v>3.743689320388349</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3409,7 +3409,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>63.16034985422741</v>
+        <v>63.12330097087379</v>
       </c>
     </row>
   </sheetData>
@@ -3444,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.03336572724327826</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3452,7 +3452,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1316812439261419</v>
+        <v>0.1318770226537217</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2094266277939748</v>
+        <v>0.2095469255663431</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3468,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.2619047619047619</v>
+        <v>0.2619741100323625</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3476,7 +3476,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3284742468415938</v>
+        <v>0.3284789644012945</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3487,7 +3487,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.06705539358600583</v>
+        <v>0.06699029126213592</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3495,7 +3495,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2623906705539358</v>
+        <v>0.2631067961165048</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3503,7 +3503,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.4003887269193392</v>
+        <v>0.4009708737864078</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3511,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.4732750242954324</v>
+        <v>0.4737864077669903</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3519,7 +3519,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.5568513119533528</v>
+        <v>0.5572815533980583</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3527,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>6.728862973760933</v>
+        <v>6.724271844660194</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3535,7 +3535,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>59.1175898931001</v>
+        <v>59.06796116504854</v>
       </c>
     </row>
   </sheetData>
@@ -3570,7 +3570,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.08373825720764495</v>
+        <v>0.08365695792880258</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3578,7 +3578,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2452218982831228</v>
+        <v>0.2454692556634304</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3586,7 +3586,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.4029802397149336</v>
+        <v>0.4030744336569579</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3594,7 +3594,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4792678976352445</v>
+        <v>0.4792880258899677</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3602,7 +3602,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5249433106575965</v>
+        <v>0.5249190938511328</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3613,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1681243926141885</v>
+        <v>0.1679611650485437</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3621,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4897959183673469</v>
+        <v>0.4902912621359223</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3629,7 +3629,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7968901846452867</v>
+        <v>0.7970873786407767</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3637,7 +3637,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.9057337220602527</v>
+        <v>0.9058252427184466</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3645,7 +3645,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.93488824101069</v>
+        <v>0.9349514563106797</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3653,7 +3653,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>3.171039844509232</v>
+        <v>3.169902912621359</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3661,7 +3661,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>59.92322643343051</v>
+        <v>59.8747572815534</v>
       </c>
     </row>
   </sheetData>
@@ -3704,7 +3704,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.00826044703595724</v>
+        <v>0.00825242718446602</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3712,7 +3712,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.03822481373501782</v>
+        <v>0.03818770226537217</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3720,7 +3720,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.0785552316164561</v>
+        <v>0.07880258899676375</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3728,7 +3728,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.1052802073210236</v>
+        <v>0.1055016181229773</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3747,7 +3747,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.01652089407191448</v>
+        <v>0.01650485436893204</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3755,7 +3755,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.07677356656948493</v>
+        <v>0.0766990291262136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3763,7 +3763,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.1574344023323615</v>
+        <v>0.158252427184466</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3771,7 +3771,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.2089407191448008</v>
+        <v>0.2097087378640777</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3779,7 +3779,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>15.73760932944606</v>
+        <v>15.72621359223301</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3787,7 +3787,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>81.23420796890184</v>
+        <v>81.1883495145631</v>
       </c>
     </row>
   </sheetData>
@@ -3822,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3830,7 +3830,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3838,7 +3838,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3846,7 +3846,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3854,7 +3854,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3865,7 +3865,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3873,7 +3873,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3881,7 +3881,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3889,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3897,7 +3897,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3905,7 +3905,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3913,7 +3913,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -3948,7 +3948,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05571752510528021</v>
+        <v>0.05566343042071198</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3956,7 +3956,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1243926141885325</v>
+        <v>0.1244336569579288</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3964,7 +3964,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2646582442500809</v>
+        <v>0.2645631067961165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3972,7 +3972,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3219954648526077</v>
+        <v>0.3218446601941747</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3980,7 +3980,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3399740848720441</v>
+        <v>0.3398058252427185</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3991,7 +3991,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1117589893100097</v>
+        <v>0.1116504854368932</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3999,7 +3999,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.2487852283770651</v>
+        <v>0.2485436893203883</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4007,7 +4007,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.5238095238095238</v>
+        <v>0.5233009708737864</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4015,7 +4015,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.6209912536443148</v>
+        <v>0.6203883495145631</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4023,7 +4023,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.6297376093294461</v>
+        <v>0.629126213592233</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4031,7 +4031,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>38.41010689990282</v>
+        <v>38.38640776699029</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4039,7 +4039,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>170.9650145772595</v>
+        <v>170.8553398058253</v>
       </c>
     </row>
   </sheetData>
@@ -4074,7 +4074,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.06397797214123746</v>
+        <v>0.06391585760517798</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4082,7 +4082,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2055393586005831</v>
+        <v>0.2058252427184466</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4090,7 +4090,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3564949789439585</v>
+        <v>0.3566343042071198</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4098,7 +4098,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4177194687398768</v>
+        <v>0.4177993527508091</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4106,7 +4106,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.4512471655328797</v>
+        <v>0.451294498381877</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4117,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.1282798833819242</v>
+        <v>0.1281553398058252</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4125,7 +4125,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.4120505344995141</v>
+        <v>0.412621359223301</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4133,7 +4133,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.7084548104956269</v>
+        <v>0.7087378640776699</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4141,7 +4141,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.8134110787172012</v>
+        <v>0.8135922330097087</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4149,7 +4149,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.8658892128279884</v>
+        <v>0.8660194174757282</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4157,7 +4157,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>4.624878522837706</v>
+        <v>4.622330097087379</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4165,7 +4165,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>81.25364431486881</v>
+        <v>81.19805825242719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update experimental results for multiple bugs
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/Summary/All/multiple_bugs_2bug.xlsx
+++ b/experiment_results/SBFL_ONLY/Summary/All/multiple_bugs_2bug.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="10">
   <si>
     <t>EVALUATION_METRIC</t>
   </si>
@@ -60,10 +60,19 @@
     <t>Proportion of cases that found bugs</t>
   </si>
   <si>
+    <t>Num of cases that found bugs (Hit@x)</t>
+  </si>
+  <si>
     <t>Best rank</t>
   </si>
   <si>
     <t>Worst rank</t>
+  </si>
+  <si>
+    <t>Best exam</t>
+  </si>
+  <si>
+    <t>Worst exam</t>
   </si>
 </sst>
 </file>
@@ -395,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1328478964401294</v>
+        <v>0.1330097087378641</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -436,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2105177993527508</v>
+        <v>0.2106796116504855</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -444,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.2624595469255664</v>
+        <v>0.262621359223301</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -452,7 +461,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3297734627831715</v>
+        <v>0.3299352750809061</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -502,16 +511,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>6.712621359223301</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>59.06310679611651</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>3.312063720505753</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>12.74100532004786</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +589,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -570,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4783171521035599</v>
+        <v>0.4783171521035598</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -628,16 +696,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.381553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>56.81553398058252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.599097526848665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.53168187266877</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +774,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -696,7 +823,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4783171521035599</v>
+        <v>0.4783171521035598</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -754,16 +881,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.433980582524272</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>51.0757281553398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.648546127485662</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.24331356963751</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +959,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -822,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4711974110032363</v>
+        <v>0.4711974110032362</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -830,7 +1016,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.526051779935275</v>
+        <v>0.5260517799352751</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -880,16 +1066,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>6.567961165048544</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>74.80291262135923</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2.220445092185002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>14.11620024725235</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +1144,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -948,7 +1193,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4711974110032363</v>
+        <v>0.4711974110032362</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -956,7 +1201,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.526051779935275</v>
+        <v>0.5260517799352751</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1006,16 +1251,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>6.567961165048544</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>74.80291262135923</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2.220445092185002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>14.11620024725235</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1329,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1074,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4807443365695793</v>
+        <v>0.4807443365695792</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1132,16 +1436,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.133009708737864</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>52.2368932038835</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.489515122386936</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.62628961232893</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1514,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1176,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.0517799352750809</v>
+        <v>0.05177993527508091</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1192,7 +1555,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.28915857605178</v>
+        <v>0.2891585760517799</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1200,7 +1563,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3425566343042071</v>
+        <v>0.342556634304207</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1208,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3673139158576052</v>
+        <v>0.3673139158576051</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1258,16 +1621,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>4.890291262135922</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>70.36504854368933</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2.165822517858836</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>16.02976832310655</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1699,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1326,7 +1748,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.07880258899676375</v>
+        <v>0.07896440129449837</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1334,7 +1756,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.1055016181229773</v>
+        <v>0.105663430420712</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1384,16 +1806,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>15.72621359223301</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>81.1883495145631</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>6.428204055196468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>19.72931423469107</v>
       </c>
     </row>
   </sheetData>
@@ -1403,7 +1884,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1428,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1436,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1444,7 +1925,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1452,7 +1933,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1460,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1510,16 +1991,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +2069,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1578,7 +2118,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4783171521035599</v>
+        <v>0.4783171521035598</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1636,16 +2176,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.381553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>56.81553398058252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.599097526848665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.53168187266877</v>
       </c>
     </row>
   </sheetData>
@@ -1655,7 +2254,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1704,7 +2303,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4783171521035599</v>
+        <v>0.4783171521035598</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1762,16 +2361,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.381553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>56.81553398058252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.599097526848665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.53168187266877</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +2439,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1830,7 +2488,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4841423948220065</v>
+        <v>0.4841423948220064</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1888,16 +2546,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.112621359223301</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>57.92912621359223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.479107054602467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>12.00649692684191</v>
       </c>
     </row>
   </sheetData>
@@ -1907,7 +2624,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1932,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1940,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1948,7 +2665,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1956,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1964,7 +2681,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2014,16 +2731,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -2033,7 +2809,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2058,7 +2834,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2066,7 +2842,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2074,7 +2850,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2082,7 +2858,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2090,7 +2866,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2140,16 +2916,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2994,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2184,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2192,7 +3027,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2200,7 +3035,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2208,7 +3043,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2216,7 +3051,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2266,16 +3101,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -2285,7 +3179,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2342,7 +3236,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3488673139158576</v>
+        <v>0.3488673139158575</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2392,16 +3286,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>6.301941747572815</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>62.74660194174757</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2.948092865787706</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>14.02130071399982</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +3364,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2436,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.07977346278317153</v>
+        <v>0.07977346278317152</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2460,7 +3413,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4681229773462783</v>
+        <v>0.4681229773462782</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2468,7 +3421,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5186084142394822</v>
+        <v>0.5186084142394821</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2518,16 +3471,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.181553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>65.10582524271845</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.57361226682466</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>13.35315704331389</v>
       </c>
     </row>
   </sheetData>
@@ -2537,7 +3549,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2562,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2570,7 +3582,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2578,7 +3590,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2586,7 +3598,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2594,7 +3606,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2644,16 +3656,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -2663,7 +3734,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2704,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3978964401294499</v>
+        <v>0.3978964401294498</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2712,7 +3783,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4707119741100324</v>
+        <v>0.4707119741100323</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2770,16 +3841,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>6.298058252427184</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>80.02427184466019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.983689620619697</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>15.23012050335801</v>
       </c>
     </row>
   </sheetData>
@@ -2789,7 +3919,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2838,7 +3968,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4783171521035599</v>
+        <v>0.4783171521035598</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2896,16 +4026,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.381553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>56.81553398058252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.599097526848665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.53168187266877</v>
       </c>
     </row>
   </sheetData>
@@ -2915,7 +4104,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2964,7 +4153,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4783171521035599</v>
+        <v>0.4783171521035598</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3022,16 +4211,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.381553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>56.81553398058252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.599097526848665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>11.53168187266877</v>
       </c>
     </row>
   </sheetData>
@@ -3041,7 +4289,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3066,7 +4314,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.07977346278317153</v>
+        <v>0.07977346278317152</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3090,7 +4338,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4681229773462783</v>
+        <v>0.4681229773462782</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3098,7 +4346,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.5181229773462784</v>
+        <v>0.5181229773462783</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3148,16 +4396,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.181553398058252</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>54.49320388349515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.57361226682466</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>12.38180117310184</v>
       </c>
     </row>
   </sheetData>
@@ -3167,7 +4474,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3216,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.1605177993527508</v>
+        <v>0.1606796116504854</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3224,7 +4531,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.1920711974110033</v>
+        <v>0.1922330097087379</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3274,16 +4581,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>9.133009708737864</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>57.0378640776699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>3.839563334041333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>15.03539732490117</v>
       </c>
     </row>
   </sheetData>
@@ -3293,7 +4659,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3318,7 +4684,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.07831715210355987</v>
+        <v>0.07831715210355986</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3342,7 +4708,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4501618122977347</v>
+        <v>0.4501618122977346</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3350,7 +4716,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.4826860841423948</v>
+        <v>0.4826860841423947</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3400,16 +4766,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.743689320388349</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>63.12330097087379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.77436165301155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>13.98023793121739</v>
       </c>
     </row>
   </sheetData>
@@ -3419,7 +4844,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3452,7 +4877,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1318770226537217</v>
+        <v>0.1320388349514563</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3460,7 +4885,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2095469255663431</v>
+        <v>0.2097087378640777</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3468,7 +4893,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.2619741100323625</v>
+        <v>0.2621359223300971</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3476,7 +4901,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3284789644012945</v>
+        <v>0.3286407766990291</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3526,16 +4951,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>6.724271844660194</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>59.06796116504854</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>3.315589748848023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>12.74259409064707</v>
       </c>
     </row>
   </sheetData>
@@ -3545,7 +5029,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3594,7 +5078,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4792880258899677</v>
+        <v>0.4792880258899676</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3652,16 +5136,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>3.169902912621359</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>59.8747572815534</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.463291490696731</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>12.55710818585553</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +5214,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3720,7 +5263,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.07880258899676375</v>
+        <v>0.07896440129449837</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3728,7 +5271,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.1055016181229773</v>
+        <v>0.105663430420712</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3778,16 +5321,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>15.72621359223301</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>81.1883495145631</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>6.428204055196468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>19.72931423469107</v>
       </c>
     </row>
   </sheetData>
@@ -3797,7 +5399,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3822,7 +5424,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3830,7 +5432,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3838,7 +5440,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3846,7 +5448,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3854,7 +5456,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3904,16 +5506,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -3923,7 +5584,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3948,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05566343042071198</v>
+        <v>0.05566343042071197</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3956,7 +5617,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1244336569579288</v>
+        <v>0.1242718446601942</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3964,7 +5625,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.2645631067961165</v>
+        <v>0.2644012944983818</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3972,7 +5633,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3218446601941747</v>
+        <v>0.3216828478964401</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3980,7 +5641,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.3398058252427185</v>
+        <v>0.3396440129449838</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4030,16 +5691,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>38.38640776699029</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>170.8553398058253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.936259574263456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>33.87693209773436</v>
       </c>
     </row>
   </sheetData>
@@ -4049,7 +5769,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4074,7 +5794,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.06391585760517798</v>
+        <v>0.063915857605178</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4090,7 +5810,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3566343042071198</v>
+        <v>0.3566343042071197</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4098,7 +5818,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.4177993527508091</v>
+        <v>0.417799352750809</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4156,16 +5876,75 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
         <v>4.622330097087379</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>81.19805825242719</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1.724702265196487</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>18.02277072204123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>